<commit_message>
update new LED layout
</commit_message>
<xml_diff>
--- a/file/LED-Layout.xlsx
+++ b/file/LED-Layout.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>X</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t>L04</t>
+  </si>
+  <si>
+    <t>L05</t>
+  </si>
+  <si>
+    <t>L06</t>
   </si>
 </sst>
 </file>
@@ -479,7 +485,7 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5">
-        <v>340.50299999999999</v>
+        <v>325.50299999999999</v>
       </c>
       <c r="C2" s="5">
         <v>83.510999999999996</v>
@@ -496,18 +502,18 @@
         <v>4</v>
       </c>
       <c r="B3" s="9">
-        <v>136.52000000000001</v>
+        <v>136.45400000000001</v>
       </c>
       <c r="C3" s="9">
-        <v>70.319999999999993</v>
+        <v>56.89</v>
       </c>
       <c r="D3" s="10">
         <f t="shared" ref="D3:D6" si="0">D$2/B$2*B3</f>
-        <v>89.809722674983789</v>
+        <v>93.902962491897171</v>
       </c>
       <c r="E3" s="10">
         <f t="shared" ref="E3:E6" si="1">E$2/C$2*C3</f>
-        <v>53.890864676509679</v>
+        <v>43.598567853336689</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -515,35 +521,35 @@
         <v>5</v>
       </c>
       <c r="B4" s="9">
-        <v>136.52000000000001</v>
+        <v>136.45400000000001</v>
       </c>
       <c r="C4" s="9">
-        <v>75.319999999999993</v>
+        <v>59.79</v>
       </c>
       <c r="D4" s="10">
         <f t="shared" si="0"/>
-        <v>89.809722674983789</v>
+        <v>93.902962491897171</v>
       </c>
       <c r="E4" s="10">
         <f t="shared" si="1"/>
-        <v>57.722695213804165</v>
+        <v>45.821029564967489</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="11">
-        <v>183.93799999999999</v>
-      </c>
-      <c r="C5" s="11">
+      <c r="B5" s="9">
+        <v>136.45400000000001</v>
+      </c>
+      <c r="C5" s="9">
         <v>70.319999999999993</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="10">
         <f t="shared" si="0"/>
-        <v>121.00366810277735</v>
-      </c>
-      <c r="E5" s="12">
+        <v>93.902962491897171</v>
+      </c>
+      <c r="E5" s="10">
         <f t="shared" si="1"/>
         <v>53.890864676509679</v>
       </c>
@@ -553,33 +559,57 @@
         <v>7</v>
       </c>
       <c r="B6" s="11">
-        <v>183.93799999999999</v>
+        <v>189.04900000000001</v>
       </c>
       <c r="C6" s="11">
-        <v>75.319999999999993</v>
+        <v>56.89</v>
       </c>
       <c r="D6" s="12">
         <f t="shared" si="0"/>
-        <v>121.00366810277735</v>
+        <v>130.09703750810286</v>
       </c>
       <c r="E6" s="12">
         <f t="shared" si="1"/>
-        <v>57.722695213804165</v>
+        <v>43.598567853336689</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="A7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="11">
+        <v>189.04900000000001</v>
+      </c>
+      <c r="C7" s="11">
+        <v>59.79</v>
+      </c>
+      <c r="D7" s="12">
+        <f t="shared" ref="D7:D8" si="2">D$2/B$2*B7</f>
+        <v>130.09703750810286</v>
+      </c>
+      <c r="E7" s="12">
+        <f t="shared" ref="E7:E8" si="3">E$2/C$2*C7</f>
+        <v>45.821029564967489</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="A8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="11">
+        <v>189.04900000000001</v>
+      </c>
+      <c r="C8" s="11">
+        <v>62.69</v>
+      </c>
+      <c r="D8" s="12">
+        <f t="shared" si="2"/>
+        <v>130.09703750810286</v>
+      </c>
+      <c r="E8" s="12">
+        <f t="shared" si="3"/>
+        <v>48.043491276598296</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>

</xml_diff>